<commit_message>
nos vanmos perri :d
</commit_message>
<xml_diff>
--- a/resultados.xlsx
+++ b/resultados.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,89 +424,18 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Archivo</t>
+          <t>Pregunta</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Pregunta</t>
+          <t>Respuesta</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Conteo</t>
         </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Documento_2024-06-17_143254.pdf</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Documento_2024-06-17_143254.pdf</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
este funciona, falta ajustar el conteo y la posicion del numero
</commit_message>
<xml_diff>
--- a/resultados.xlsx
+++ b/resultados.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,6 +438,66 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Pregunta1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>(100, 50)</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Pregunta1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>(200, 80)</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Pregunta2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>(150, 60)</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Pregunta2</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>(250, 90)</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>